<commit_message>
Remove Duplicates (Data-Data Tool-Remove Duplicates)
</commit_message>
<xml_diff>
--- a/Excel/Data Cleaning Excel Tutorial.xlsx
+++ b/Excel/Data Cleaning Excel Tutorial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milo4\Desktop\DataAnalysisLearning\Data-Analysis-Portfolio-Projects\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECFB9EFC-1E61-4BBF-B231-9DA9EC4C620A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE84C488-C1EA-4B2E-AF21-F785F6A119C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="137">
   <si>
     <t>S.No.</t>
   </si>
@@ -1299,7 +1299,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2641,25 +2641,25 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B47">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C47" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="D47" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="E47" t="s">
-        <v>26</v>
+        <v>132</v>
       </c>
       <c r="F47" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="G47" s="4">
-        <v>395000</v>
+        <v>405000</v>
       </c>
       <c r="H47" s="2">
         <v>44391</v>
@@ -2669,33 +2669,7 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48">
-        <v>44</v>
-      </c>
-      <c r="B48">
-        <v>45</v>
-      </c>
-      <c r="C48" t="s">
-        <v>128</v>
-      </c>
-      <c r="D48" t="s">
-        <v>129</v>
-      </c>
-      <c r="E48" t="s">
-        <v>132</v>
-      </c>
-      <c r="F48" t="s">
-        <v>130</v>
-      </c>
-      <c r="G48" s="4">
-        <v>405000</v>
-      </c>
-      <c r="H48" s="2">
-        <v>44391</v>
-      </c>
-      <c r="I48" s="2">
-        <v>43862</v>
-      </c>
+      <c r="G48"/>
     </row>
   </sheetData>
   <dataConsolidate/>

</xml_diff>

<commit_message>
President column fixed with PROPER function (first name and last name capitalized)
</commit_message>
<xml_diff>
--- a/Excel/Data Cleaning Excel Tutorial.xlsx
+++ b/Excel/Data Cleaning Excel Tutorial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milo4\Desktop\DataAnalysisLearning\Data-Analysis-Portfolio-Projects\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE84C488-C1EA-4B2E-AF21-F785F6A119C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE2B5A9-1D24-44CA-B8D5-209AADCBBD13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="138">
   <si>
     <t>S.No.</t>
   </si>
@@ -443,6 +443,9 @@
   </si>
   <si>
     <t>date updated</t>
+  </si>
+  <si>
+    <t>President-fixed</t>
   </si>
 </sst>
 </file>
@@ -595,7 +598,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -773,6 +776,18 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -936,12 +951,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1297,44 +1314,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="23.5546875" style="3"/>
+    <col min="8" max="8" width="23.5546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>136</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1344,26 +1364,30 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="5" t="str">
+        <f>PROPER(C2)</f>
+        <v>George Washington</v>
+      </c>
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>131</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="4">
+      <c r="H2" s="4">
         <v>5000</v>
       </c>
-      <c r="H2" s="1">
-        <v>44391</v>
-      </c>
       <c r="I2" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J2" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1373,26 +1397,30 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="5" t="str">
+        <f t="shared" ref="D3:D47" si="0">PROPER(C3)</f>
+        <v>John Adams</v>
+      </c>
+      <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="4">
+      <c r="H3" s="4">
         <v>10000</v>
       </c>
-      <c r="H3" s="1">
-        <v>44391</v>
-      </c>
       <c r="I3" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J3" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1402,26 +1430,30 @@
       <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Thomas Jefferson</v>
+      </c>
+      <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>13</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="4">
+      <c r="H4" s="4">
         <v>15000</v>
       </c>
-      <c r="H4" s="1">
-        <v>44391</v>
-      </c>
       <c r="I4" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J4" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1431,26 +1463,30 @@
       <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>James Madison</v>
+      </c>
+      <c r="E5" t="s">
         <v>16</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>13</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="4">
+      <c r="H5" s="4">
         <v>20000</v>
       </c>
-      <c r="H5" s="1">
-        <v>44391</v>
-      </c>
       <c r="I5" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J5" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1460,26 +1496,30 @@
       <c r="C6" t="s">
         <v>18</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>James Monroe</v>
+      </c>
+      <c r="E6" t="s">
         <v>19</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>13</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="4">
+      <c r="H6" s="4">
         <v>25000</v>
       </c>
-      <c r="H6" s="1">
-        <v>44391</v>
-      </c>
       <c r="I6" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J6" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1489,26 +1529,30 @@
       <c r="C7" t="s">
         <v>21</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>John Quincy Adams</v>
+      </c>
+      <c r="E7" t="s">
         <v>22</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>13</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="4">
+      <c r="H7" s="4">
         <v>30000</v>
       </c>
-      <c r="H7" s="1">
-        <v>44391</v>
-      </c>
       <c r="I7" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J7" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1518,26 +1562,30 @@
       <c r="C8" t="s">
         <v>24</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Andrew Jackson</v>
+      </c>
+      <c r="E8" t="s">
         <v>25</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>26</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="4">
+      <c r="H8" s="4">
         <v>35000</v>
       </c>
-      <c r="H8" s="1">
-        <v>44391</v>
-      </c>
       <c r="I8" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J8" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1547,26 +1595,30 @@
       <c r="C9" t="s">
         <v>28</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Martin Van Buren</v>
+      </c>
+      <c r="E9" t="s">
         <v>29</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>26</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="4">
+      <c r="H9" s="4">
         <v>40000</v>
       </c>
-      <c r="H9" s="1">
-        <v>44391</v>
-      </c>
       <c r="I9" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J9" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1576,26 +1628,30 @@
       <c r="C10" t="s">
         <v>31</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>William Henry Harrison</v>
+      </c>
+      <c r="E10" t="s">
         <v>32</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>33</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="4">
+      <c r="H10" s="4">
         <v>45000</v>
       </c>
-      <c r="H10" s="1">
-        <v>44391</v>
-      </c>
       <c r="I10" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J10" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1605,26 +1661,30 @@
       <c r="C11" t="s">
         <v>35</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>John Tyler</v>
+      </c>
+      <c r="E11" t="s">
         <v>36</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>37</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>38</v>
       </c>
-      <c r="G11" s="4">
+      <c r="H11" s="4">
         <v>50000</v>
       </c>
-      <c r="H11" s="1">
-        <v>44391</v>
-      </c>
       <c r="I11" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J11" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1634,26 +1694,30 @@
       <c r="C12" t="s">
         <v>39</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>James K. Polk</v>
+      </c>
+      <c r="E12" t="s">
         <v>40</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>26</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="4">
+      <c r="H12" s="4">
         <v>55000</v>
       </c>
-      <c r="H12" s="1">
-        <v>44391</v>
-      </c>
       <c r="I12" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J12" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1663,26 +1727,30 @@
       <c r="C13" t="s">
         <v>42</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Zachary Taylor</v>
+      </c>
+      <c r="E13" t="s">
         <v>43</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>33</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>44</v>
       </c>
-      <c r="G13" s="4">
+      <c r="H13" s="4">
         <v>60000</v>
       </c>
-      <c r="H13" s="1">
-        <v>44391</v>
-      </c>
       <c r="I13" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J13" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1692,26 +1760,30 @@
       <c r="C14" t="s">
         <v>45</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Millard Fillmore</v>
+      </c>
+      <c r="E14" t="s">
         <v>46</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>33</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>38</v>
       </c>
-      <c r="G14" s="4">
+      <c r="H14" s="4">
         <v>65000</v>
       </c>
-      <c r="H14" s="1">
-        <v>44391</v>
-      </c>
       <c r="I14" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J14" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1721,26 +1793,30 @@
       <c r="C15" t="s">
         <v>47</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Franklin Pierce</v>
+      </c>
+      <c r="E15" t="s">
         <v>48</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>26</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>49</v>
       </c>
-      <c r="G15" s="4">
+      <c r="H15" s="4">
         <v>75000</v>
       </c>
-      <c r="H15" s="1">
-        <v>44391</v>
-      </c>
       <c r="I15" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J15" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1750,26 +1826,30 @@
       <c r="C16" t="s">
         <v>50</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>James Buchanan</v>
+      </c>
+      <c r="E16" t="s">
         <v>51</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>26</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>52</v>
       </c>
-      <c r="G16" s="4">
+      <c r="H16" s="4">
         <v>85000</v>
       </c>
-      <c r="H16" s="1">
-        <v>44391</v>
-      </c>
       <c r="I16" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J16" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1779,26 +1859,30 @@
       <c r="C17" t="s">
         <v>53</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Abraham Lincoln</v>
+      </c>
+      <c r="E17" t="s">
         <v>54</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>60</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>55</v>
       </c>
-      <c r="G17" s="4">
+      <c r="H17" s="4">
         <v>95000</v>
       </c>
-      <c r="H17" s="1">
-        <v>44391</v>
-      </c>
       <c r="I17" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J17" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1808,26 +1892,30 @@
       <c r="C18" t="s">
         <v>56</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Andrew Johnson</v>
+      </c>
+      <c r="E18" t="s">
         <v>57</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>26</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>38</v>
       </c>
-      <c r="G18" s="4">
+      <c r="H18" s="4">
         <v>105000</v>
       </c>
-      <c r="H18" s="1">
-        <v>44391</v>
-      </c>
       <c r="I18" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J18" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1837,26 +1925,30 @@
       <c r="C19" t="s">
         <v>58</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Ulysses S. Grant</v>
+      </c>
+      <c r="E19" t="s">
         <v>59</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>60</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>61</v>
       </c>
-      <c r="G19" s="4">
+      <c r="H19" s="4">
         <v>115000</v>
       </c>
-      <c r="H19" s="1">
-        <v>44391</v>
-      </c>
       <c r="I19" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J19" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1866,26 +1958,30 @@
       <c r="C20" t="s">
         <v>62</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Rutherford B. Hayes</v>
+      </c>
+      <c r="E20" t="s">
         <v>63</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>60</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>64</v>
       </c>
-      <c r="G20" s="4">
+      <c r="H20" s="4">
         <v>125000</v>
       </c>
-      <c r="H20" s="1">
-        <v>44391</v>
-      </c>
       <c r="I20" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J20" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1895,26 +1991,30 @@
       <c r="C21" t="s">
         <v>65</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>James A. Garfield</v>
+      </c>
+      <c r="E21" t="s">
         <v>66</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>60</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>67</v>
       </c>
-      <c r="G21" s="4">
+      <c r="H21" s="4">
         <v>135000</v>
       </c>
-      <c r="H21" s="1">
-        <v>44391</v>
-      </c>
       <c r="I21" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J21" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1924,26 +2024,30 @@
       <c r="C22" t="s">
         <v>67</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Chester A. Arthur</v>
+      </c>
+      <c r="E22" t="s">
         <v>68</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>60</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>38</v>
       </c>
-      <c r="G22" s="4">
+      <c r="H22" s="4">
         <v>145000</v>
       </c>
-      <c r="H22" s="1">
-        <v>44391</v>
-      </c>
       <c r="I22" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J22" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1953,26 +2057,30 @@
       <c r="C23" t="s">
         <v>69</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Grover Cleveland</v>
+      </c>
+      <c r="E23" t="s">
         <v>70</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>26</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>71</v>
       </c>
-      <c r="G23" s="4">
+      <c r="H23" s="4">
         <v>155000</v>
       </c>
-      <c r="H23" s="1">
-        <v>44391</v>
-      </c>
       <c r="I23" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J23" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1982,26 +2090,30 @@
       <c r="C24" t="s">
         <v>72</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Benjamin Harrison</v>
+      </c>
+      <c r="E24" t="s">
         <v>73</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>60</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>74</v>
       </c>
-      <c r="G24" s="4">
+      <c r="H24" s="4">
         <v>165000</v>
       </c>
-      <c r="H24" s="1">
-        <v>44391</v>
-      </c>
       <c r="I24" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J24" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2011,26 +2123,30 @@
       <c r="C25" t="s">
         <v>69</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Grover Cleveland</v>
+      </c>
+      <c r="E25" t="s">
         <v>75</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>26</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>76</v>
       </c>
-      <c r="G25" s="4">
+      <c r="H25" s="4">
         <v>175000</v>
       </c>
-      <c r="H25" s="1">
-        <v>44391</v>
-      </c>
       <c r="I25" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J25" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2040,26 +2156,30 @@
       <c r="C26" t="s">
         <v>77</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>William Mckinley</v>
+      </c>
+      <c r="E26" t="s">
         <v>78</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>60</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>79</v>
       </c>
-      <c r="G26" s="4">
+      <c r="H26" s="4">
         <v>185000</v>
       </c>
-      <c r="H26" s="1">
-        <v>44391</v>
-      </c>
       <c r="I26" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J26" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2069,26 +2189,30 @@
       <c r="C27" t="s">
         <v>80</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Theodore Roosevelt</v>
+      </c>
+      <c r="E27" t="s">
         <v>81</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>60</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>38</v>
       </c>
-      <c r="G27" s="4">
+      <c r="H27" s="4">
         <v>195000</v>
       </c>
-      <c r="H27" s="1">
-        <v>44391</v>
-      </c>
       <c r="I27" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J27" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2098,26 +2222,30 @@
       <c r="C28" t="s">
         <v>82</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>William Howard Taft</v>
+      </c>
+      <c r="E28" t="s">
         <v>83</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>60</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>84</v>
       </c>
-      <c r="G28" s="4">
+      <c r="H28" s="4">
         <v>205000</v>
       </c>
-      <c r="H28" s="1">
-        <v>44391</v>
-      </c>
       <c r="I28" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J28" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2127,26 +2255,30 @@
       <c r="C29" t="s">
         <v>85</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Woodrow Wilson</v>
+      </c>
+      <c r="E29" t="s">
         <v>86</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>26</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>87</v>
       </c>
-      <c r="G29" s="4">
+      <c r="H29" s="4">
         <v>225000</v>
       </c>
-      <c r="H29" s="1">
-        <v>44391</v>
-      </c>
       <c r="I29" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J29" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>27</v>
       </c>
@@ -2156,26 +2288,30 @@
       <c r="C30" t="s">
         <v>85</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Woodrow Wilson</v>
+      </c>
+      <c r="E30" t="s">
         <v>86</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>133</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>87</v>
       </c>
-      <c r="G30" s="4">
+      <c r="H30" s="4">
         <v>225000</v>
       </c>
-      <c r="H30" s="1">
-        <v>44391</v>
-      </c>
       <c r="I30" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J30" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>28</v>
       </c>
@@ -2185,26 +2321,30 @@
       <c r="C31" t="s">
         <v>88</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Warren G. Harding</v>
+      </c>
+      <c r="E31" t="s">
         <v>89</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>60</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>90</v>
       </c>
-      <c r="G31" s="4">
+      <c r="H31" s="4">
         <v>235000</v>
       </c>
-      <c r="H31" s="1">
-        <v>44391</v>
-      </c>
       <c r="I31" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J31" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>29</v>
       </c>
@@ -2214,26 +2354,30 @@
       <c r="C32" t="s">
         <v>90</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Calvin Coolidge</v>
+      </c>
+      <c r="E32" t="s">
         <v>91</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>60</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>38</v>
       </c>
-      <c r="G32" s="4">
+      <c r="H32" s="4">
         <v>245000</v>
       </c>
-      <c r="H32" s="1">
-        <v>44391</v>
-      </c>
       <c r="I32" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J32" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>30</v>
       </c>
@@ -2243,26 +2387,30 @@
       <c r="C33" t="s">
         <v>92</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Herbert Hoover</v>
+      </c>
+      <c r="E33" t="s">
         <v>93</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>60</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>94</v>
       </c>
-      <c r="G33" s="4">
+      <c r="H33" s="4">
         <v>255000</v>
       </c>
-      <c r="H33" s="1">
-        <v>44391</v>
-      </c>
       <c r="I33" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J33" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>31</v>
       </c>
@@ -2272,26 +2420,30 @@
       <c r="C34" t="s">
         <v>95</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Franklin D. Roosevelt</v>
+      </c>
+      <c r="E34" t="s">
         <v>96</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>26</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>97</v>
       </c>
-      <c r="G34" s="4">
+      <c r="H34" s="4">
         <v>265000</v>
       </c>
-      <c r="H34" s="1">
-        <v>44391</v>
-      </c>
       <c r="I34" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J34" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>32</v>
       </c>
@@ -2301,26 +2453,30 @@
       <c r="C35" t="s">
         <v>98</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Harry S. Truman</v>
+      </c>
+      <c r="E35" t="s">
         <v>99</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>26</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>38</v>
       </c>
-      <c r="G35" s="4">
+      <c r="H35" s="4">
         <v>275000</v>
       </c>
-      <c r="H35" s="1">
-        <v>44391</v>
-      </c>
       <c r="I35" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J35" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>33</v>
       </c>
@@ -2330,26 +2486,30 @@
       <c r="C36" t="s">
         <v>100</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Dwight D. Eisenhower</v>
+      </c>
+      <c r="E36" t="s">
         <v>101</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>60</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>102</v>
       </c>
-      <c r="G36" s="4">
+      <c r="H36" s="4">
         <v>285000</v>
       </c>
-      <c r="H36" s="1">
-        <v>44391</v>
-      </c>
       <c r="I36" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J36" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>34</v>
       </c>
@@ -2359,26 +2519,30 @@
       <c r="C37" t="s">
         <v>103</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>John F. Kennedy</v>
+      </c>
+      <c r="E37" t="s">
         <v>104</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>26</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>105</v>
       </c>
-      <c r="G37" s="4">
+      <c r="H37" s="4">
         <v>295000</v>
       </c>
-      <c r="H37" s="1">
-        <v>44391</v>
-      </c>
       <c r="I37" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J37" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>35</v>
       </c>
@@ -2388,26 +2552,30 @@
       <c r="C38" t="s">
         <v>105</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Lyndon B. Johnson</v>
+      </c>
+      <c r="E38" t="s">
         <v>106</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>26</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>38</v>
       </c>
-      <c r="G38" s="4">
+      <c r="H38" s="4">
         <v>305000</v>
       </c>
-      <c r="H38" s="1">
-        <v>44391</v>
-      </c>
       <c r="I38" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J38" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>36</v>
       </c>
@@ -2417,26 +2585,30 @@
       <c r="C39" t="s">
         <v>102</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Richard Nixon</v>
+      </c>
+      <c r="E39" t="s">
         <v>107</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>60</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>108</v>
       </c>
-      <c r="G39" s="4">
+      <c r="H39" s="4">
         <v>315000</v>
       </c>
-      <c r="H39" s="1">
-        <v>44391</v>
-      </c>
       <c r="I39" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J39" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>37</v>
       </c>
@@ -2446,26 +2618,30 @@
       <c r="C40" t="s">
         <v>109</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Gerald Ford</v>
+      </c>
+      <c r="E40" t="s">
         <v>110</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F40" t="s">
         <v>60</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>38</v>
       </c>
-      <c r="G40" s="4">
+      <c r="H40" s="4">
         <v>325000</v>
       </c>
-      <c r="H40" s="1">
-        <v>44391</v>
-      </c>
       <c r="I40" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J40" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>38</v>
       </c>
@@ -2475,26 +2651,30 @@
       <c r="C41" t="s">
         <v>111</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Jimmy Carter</v>
+      </c>
+      <c r="E41" t="s">
         <v>112</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F41" t="s">
         <v>26</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>113</v>
       </c>
-      <c r="G41" s="4">
+      <c r="H41" s="4">
         <v>335000</v>
       </c>
-      <c r="H41" s="1">
-        <v>44391</v>
-      </c>
       <c r="I41" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J41" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>39</v>
       </c>
@@ -2504,26 +2684,30 @@
       <c r="C42" t="s">
         <v>114</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Ronald Reagan</v>
+      </c>
+      <c r="E42" t="s">
         <v>115</v>
       </c>
-      <c r="E42" t="s">
+      <c r="F42" t="s">
         <v>60</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>116</v>
       </c>
-      <c r="G42" s="4">
+      <c r="H42" s="4">
         <v>345000</v>
       </c>
-      <c r="H42" s="1">
-        <v>44391</v>
-      </c>
       <c r="I42" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J42" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>40</v>
       </c>
@@ -2533,26 +2717,30 @@
       <c r="C43" t="s">
         <v>116</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>George H. W. Bush</v>
+      </c>
+      <c r="E43" t="s">
         <v>117</v>
       </c>
-      <c r="E43" t="s">
+      <c r="F43" t="s">
         <v>60</v>
       </c>
-      <c r="F43" t="s">
+      <c r="G43" t="s">
         <v>118</v>
       </c>
-      <c r="G43" s="4">
+      <c r="H43" s="4">
         <v>355000</v>
       </c>
-      <c r="H43" s="1">
-        <v>44391</v>
-      </c>
       <c r="I43" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J43" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>41</v>
       </c>
@@ -2562,26 +2750,30 @@
       <c r="C44" t="s">
         <v>119</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Bill Clinton</v>
+      </c>
+      <c r="E44" t="s">
         <v>120</v>
       </c>
-      <c r="E44" t="s">
+      <c r="F44" t="s">
         <v>26</v>
       </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>121</v>
       </c>
-      <c r="G44" s="4">
+      <c r="H44" s="4">
         <v>365000</v>
       </c>
-      <c r="H44" s="1">
-        <v>44391</v>
-      </c>
       <c r="I44" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J44" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>42</v>
       </c>
@@ -2591,26 +2783,30 @@
       <c r="C45" t="s">
         <v>122</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>George W. Bush</v>
+      </c>
+      <c r="E45" t="s">
         <v>123</v>
       </c>
-      <c r="E45" t="s">
+      <c r="F45" t="s">
         <v>60</v>
       </c>
-      <c r="F45" t="s">
+      <c r="G45" t="s">
         <v>124</v>
       </c>
-      <c r="G45" s="4">
+      <c r="H45" s="4">
         <v>375000</v>
       </c>
-      <c r="H45" s="1">
-        <v>44391</v>
-      </c>
       <c r="I45" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J45" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>43</v>
       </c>
@@ -2620,26 +2816,30 @@
       <c r="C46" t="s">
         <v>125</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Barack Obama</v>
+      </c>
+      <c r="E46" t="s">
         <v>126</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F46" t="s">
         <v>26</v>
       </c>
-      <c r="F46" t="s">
+      <c r="G46" t="s">
         <v>127</v>
       </c>
-      <c r="G46" s="4">
+      <c r="H46" s="4">
         <v>395000</v>
       </c>
-      <c r="H46" s="2">
-        <v>44391</v>
-      </c>
       <c r="I46" s="2">
+        <v>44391</v>
+      </c>
+      <c r="J46" s="2">
         <v>43862</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>44</v>
       </c>
@@ -2649,27 +2849,31 @@
       <c r="C47" t="s">
         <v>128</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Donald Trump</v>
+      </c>
+      <c r="E47" t="s">
         <v>129</v>
       </c>
-      <c r="E47" t="s">
+      <c r="F47" t="s">
         <v>132</v>
       </c>
-      <c r="F47" t="s">
+      <c r="G47" t="s">
         <v>130</v>
       </c>
-      <c r="G47" s="4">
+      <c r="H47" s="4">
         <v>405000</v>
       </c>
-      <c r="H47" s="2">
-        <v>44391</v>
-      </c>
       <c r="I47" s="2">
+        <v>44391</v>
+      </c>
+      <c r="J47" s="2">
         <v>43862</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G48"/>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H48"/>
     </row>
   </sheetData>
   <dataConsolidate/>

</xml_diff>

<commit_message>
Vice column fixed using TRIM to delete unnecessary space
</commit_message>
<xml_diff>
--- a/Excel/Data Cleaning Excel Tutorial.xlsx
+++ b/Excel/Data Cleaning Excel Tutorial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milo4\Desktop\DataAnalysisLearning\Data-Analysis-Portfolio-Projects\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A85A342F-8D4C-4123-8146-9CF7BBFBCBAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED3964A-8254-4DE5-9547-35A606414823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="US_Presidents Excel Tutorial Da" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'US_Presidents Excel Tutorial Da'!$A$1:$J$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'US_Presidents Excel Tutorial Da'!$A$1:$K$47</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="137">
   <si>
     <t>S.No.</t>
   </si>
@@ -443,6 +443,9 @@
   </si>
   <si>
     <t>President-fixed</t>
+  </si>
+  <si>
+    <t>Vice-fixed</t>
   </si>
 </sst>
 </file>
@@ -595,7 +598,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -784,6 +787,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -948,7 +975,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -956,6 +983,10 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1311,18 +1342,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J48"/>
+  <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10:F11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="23.5546875" style="3"/>
+    <col min="9" max="9" width="23.5546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1335,23 +1366,26 @@
       <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="8" t="s">
         <v>3</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>134</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1368,23 +1402,27 @@
       <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="7" t="s">
         <v>130</v>
       </c>
       <c r="G2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="9" t="str">
+        <f>TRIM(G2)</f>
+        <v>John Adams</v>
+      </c>
+      <c r="I2" s="4">
         <v>5000</v>
       </c>
-      <c r="I2" s="1">
-        <v>44391</v>
-      </c>
       <c r="J2" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K2" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1401,23 +1439,27 @@
       <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="9" t="str">
+        <f t="shared" ref="H3:H47" si="1">TRIM(G3)</f>
+        <v>Thomas Jefferson</v>
+      </c>
+      <c r="I3" s="4">
         <v>10000</v>
       </c>
-      <c r="I3" s="1">
-        <v>44391</v>
-      </c>
       <c r="J3" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K3" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1434,23 +1476,27 @@
       <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G4" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>Aaron Burr</v>
+      </c>
+      <c r="I4" s="4">
         <v>15000</v>
       </c>
-      <c r="I4" s="1">
-        <v>44391</v>
-      </c>
       <c r="J4" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K4" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1467,23 +1513,27 @@
       <c r="E5" t="s">
         <v>16</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G5" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>George Clinton</v>
+      </c>
+      <c r="I5" s="4">
         <v>20000</v>
       </c>
-      <c r="I5" s="1">
-        <v>44391</v>
-      </c>
       <c r="J5" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K5" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1500,23 +1550,27 @@
       <c r="E6" t="s">
         <v>19</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G6" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>Daniel D. Tompkins</v>
+      </c>
+      <c r="I6" s="4">
         <v>25000</v>
       </c>
-      <c r="I6" s="1">
-        <v>44391</v>
-      </c>
       <c r="J6" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K6" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1533,23 +1587,27 @@
       <c r="E7" t="s">
         <v>22</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G7" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>John C. Calhoun</v>
+      </c>
+      <c r="I7" s="4">
         <v>30000</v>
       </c>
-      <c r="I7" s="1">
-        <v>44391</v>
-      </c>
       <c r="J7" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K7" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1566,23 +1624,27 @@
       <c r="E8" t="s">
         <v>25</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="7" t="s">
         <v>26</v>
       </c>
       <c r="G8" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>John C. Calhoun</v>
+      </c>
+      <c r="I8" s="4">
         <v>35000</v>
       </c>
-      <c r="I8" s="1">
-        <v>44391</v>
-      </c>
       <c r="J8" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K8" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1599,23 +1661,27 @@
       <c r="E9" t="s">
         <v>29</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="7" t="s">
         <v>26</v>
       </c>
       <c r="G9" t="s">
         <v>30</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>Richard Mentor Johnson</v>
+      </c>
+      <c r="I9" s="4">
         <v>40000</v>
       </c>
-      <c r="I9" s="1">
-        <v>44391</v>
-      </c>
       <c r="J9" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K9" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1632,23 +1698,27 @@
       <c r="E10" t="s">
         <v>32</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="7" t="s">
         <v>33</v>
       </c>
       <c r="G10" t="s">
         <v>34</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>John Tyler</v>
+      </c>
+      <c r="I10" s="4">
         <v>45000</v>
       </c>
-      <c r="I10" s="1">
-        <v>44391</v>
-      </c>
       <c r="J10" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K10" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1665,23 +1735,27 @@
       <c r="E11" t="s">
         <v>36</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="7" t="s">
         <v>33</v>
       </c>
       <c r="G11" t="s">
         <v>37</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>Office vacant</v>
+      </c>
+      <c r="I11" s="4">
         <v>50000</v>
       </c>
-      <c r="I11" s="1">
-        <v>44391</v>
-      </c>
       <c r="J11" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K11" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1698,23 +1772,27 @@
       <c r="E12" t="s">
         <v>39</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="7" t="s">
         <v>26</v>
       </c>
       <c r="G12" t="s">
         <v>40</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>George M. Dallas</v>
+      </c>
+      <c r="I12" s="4">
         <v>55000</v>
       </c>
-      <c r="I12" s="1">
-        <v>44391</v>
-      </c>
       <c r="J12" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K12" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1731,23 +1809,27 @@
       <c r="E13" t="s">
         <v>42</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="7" t="s">
         <v>33</v>
       </c>
       <c r="G13" t="s">
         <v>43</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>Millard Fillmore</v>
+      </c>
+      <c r="I13" s="4">
         <v>60000</v>
       </c>
-      <c r="I13" s="1">
-        <v>44391</v>
-      </c>
       <c r="J13" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K13" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1764,23 +1846,27 @@
       <c r="E14" t="s">
         <v>45</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="7" t="s">
         <v>33</v>
       </c>
       <c r="G14" t="s">
         <v>37</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>Office vacant</v>
+      </c>
+      <c r="I14" s="4">
         <v>65000</v>
       </c>
-      <c r="I14" s="1">
-        <v>44391</v>
-      </c>
       <c r="J14" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K14" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1797,23 +1883,27 @@
       <c r="E15" t="s">
         <v>47</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="7" t="s">
         <v>26</v>
       </c>
       <c r="G15" t="s">
         <v>48</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>William R. King</v>
+      </c>
+      <c r="I15" s="4">
         <v>75000</v>
       </c>
-      <c r="I15" s="1">
-        <v>44391</v>
-      </c>
       <c r="J15" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K15" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1830,23 +1920,27 @@
       <c r="E16" t="s">
         <v>50</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="7" t="s">
         <v>26</v>
       </c>
       <c r="G16" t="s">
         <v>51</v>
       </c>
-      <c r="H16" s="4">
+      <c r="H16" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>John C. Breckinridge</v>
+      </c>
+      <c r="I16" s="4">
         <v>85000</v>
       </c>
-      <c r="I16" s="1">
-        <v>44391</v>
-      </c>
       <c r="J16" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K16" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1863,23 +1957,27 @@
       <c r="E17" t="s">
         <v>53</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="7" t="s">
         <v>59</v>
       </c>
       <c r="G17" t="s">
         <v>54</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H17" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>Hannibal Hamlin</v>
+      </c>
+      <c r="I17" s="4">
         <v>95000</v>
       </c>
-      <c r="I17" s="1">
-        <v>44391</v>
-      </c>
       <c r="J17" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K17" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1896,23 +1994,27 @@
       <c r="E18" t="s">
         <v>56</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="7" t="s">
         <v>26</v>
       </c>
       <c r="G18" t="s">
         <v>37</v>
       </c>
-      <c r="H18" s="4">
+      <c r="H18" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>Office vacant</v>
+      </c>
+      <c r="I18" s="4">
         <v>105000</v>
       </c>
-      <c r="I18" s="1">
-        <v>44391</v>
-      </c>
       <c r="J18" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K18" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1929,23 +2031,27 @@
       <c r="E19" t="s">
         <v>58</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="7" t="s">
         <v>59</v>
       </c>
       <c r="G19" t="s">
         <v>60</v>
       </c>
-      <c r="H19" s="4">
+      <c r="H19" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>Schuyler Colfax</v>
+      </c>
+      <c r="I19" s="4">
         <v>115000</v>
       </c>
-      <c r="I19" s="1">
-        <v>44391</v>
-      </c>
       <c r="J19" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K19" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1962,23 +2068,27 @@
       <c r="E20" t="s">
         <v>62</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="7" t="s">
         <v>59</v>
       </c>
       <c r="G20" t="s">
         <v>63</v>
       </c>
-      <c r="H20" s="4">
+      <c r="H20" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>William A. Wheeler</v>
+      </c>
+      <c r="I20" s="4">
         <v>125000</v>
       </c>
-      <c r="I20" s="1">
-        <v>44391</v>
-      </c>
       <c r="J20" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K20" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1995,23 +2105,27 @@
       <c r="E21" t="s">
         <v>65</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="7" t="s">
         <v>59</v>
       </c>
       <c r="G21" t="s">
         <v>66</v>
       </c>
-      <c r="H21" s="4">
+      <c r="H21" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>Chester A. Arthur</v>
+      </c>
+      <c r="I21" s="4">
         <v>135000</v>
       </c>
-      <c r="I21" s="1">
-        <v>44391</v>
-      </c>
       <c r="J21" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K21" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2028,23 +2142,27 @@
       <c r="E22" t="s">
         <v>67</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="7" t="s">
         <v>59</v>
       </c>
       <c r="G22" t="s">
         <v>37</v>
       </c>
-      <c r="H22" s="4">
+      <c r="H22" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>Office vacant</v>
+      </c>
+      <c r="I22" s="4">
         <v>145000</v>
       </c>
-      <c r="I22" s="1">
-        <v>44391</v>
-      </c>
       <c r="J22" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K22" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2061,23 +2179,27 @@
       <c r="E23" t="s">
         <v>69</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="7" t="s">
         <v>26</v>
       </c>
       <c r="G23" t="s">
         <v>70</v>
       </c>
-      <c r="H23" s="4">
+      <c r="H23" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>Thomas A. Hendricks</v>
+      </c>
+      <c r="I23" s="4">
         <v>155000</v>
       </c>
-      <c r="I23" s="1">
-        <v>44391</v>
-      </c>
       <c r="J23" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K23" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2094,23 +2216,27 @@
       <c r="E24" t="s">
         <v>72</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="7" t="s">
         <v>59</v>
       </c>
       <c r="G24" t="s">
         <v>73</v>
       </c>
-      <c r="H24" s="4">
+      <c r="H24" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>Levi P. Morton</v>
+      </c>
+      <c r="I24" s="4">
         <v>165000</v>
       </c>
-      <c r="I24" s="1">
-        <v>44391</v>
-      </c>
       <c r="J24" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K24" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2127,23 +2253,27 @@
       <c r="E25" t="s">
         <v>74</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="7" t="s">
         <v>26</v>
       </c>
       <c r="G25" t="s">
         <v>75</v>
       </c>
-      <c r="H25" s="4">
+      <c r="H25" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>Adlai Stevenson</v>
+      </c>
+      <c r="I25" s="4">
         <v>175000</v>
       </c>
-      <c r="I25" s="1">
-        <v>44391</v>
-      </c>
       <c r="J25" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K25" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2160,23 +2290,27 @@
       <c r="E26" t="s">
         <v>77</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="7" t="s">
         <v>59</v>
       </c>
       <c r="G26" t="s">
         <v>78</v>
       </c>
-      <c r="H26" s="4">
+      <c r="H26" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>Garret Hobart</v>
+      </c>
+      <c r="I26" s="4">
         <v>185000</v>
       </c>
-      <c r="I26" s="1">
-        <v>44391</v>
-      </c>
       <c r="J26" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K26" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2193,23 +2327,27 @@
       <c r="E27" t="s">
         <v>80</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="7" t="s">
         <v>59</v>
       </c>
       <c r="G27" t="s">
         <v>37</v>
       </c>
-      <c r="H27" s="4">
+      <c r="H27" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>Office vacant</v>
+      </c>
+      <c r="I27" s="4">
         <v>195000</v>
       </c>
-      <c r="I27" s="1">
-        <v>44391</v>
-      </c>
       <c r="J27" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K27" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2226,23 +2364,27 @@
       <c r="E28" t="s">
         <v>82</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="7" t="s">
         <v>59</v>
       </c>
       <c r="G28" t="s">
         <v>83</v>
       </c>
-      <c r="H28" s="4">
+      <c r="H28" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>James S. Sherman</v>
+      </c>
+      <c r="I28" s="4">
         <v>205000</v>
       </c>
-      <c r="I28" s="1">
-        <v>44391</v>
-      </c>
       <c r="J28" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K28" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2259,23 +2401,27 @@
       <c r="E29" t="s">
         <v>85</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="7" t="s">
         <v>26</v>
       </c>
       <c r="G29" t="s">
         <v>86</v>
       </c>
-      <c r="H29" s="4">
+      <c r="H29" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>Thomas R. Marshall</v>
+      </c>
+      <c r="I29" s="4">
         <v>225000</v>
       </c>
-      <c r="I29" s="1">
-        <v>44391</v>
-      </c>
       <c r="J29" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K29" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>27</v>
       </c>
@@ -2292,23 +2438,27 @@
       <c r="E30" t="s">
         <v>85</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="7" t="s">
         <v>131</v>
       </c>
       <c r="G30" t="s">
         <v>86</v>
       </c>
-      <c r="H30" s="4">
+      <c r="H30" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>Thomas R. Marshall</v>
+      </c>
+      <c r="I30" s="4">
         <v>225000</v>
       </c>
-      <c r="I30" s="1">
-        <v>44391</v>
-      </c>
       <c r="J30" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K30" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>28</v>
       </c>
@@ -2325,23 +2475,27 @@
       <c r="E31" t="s">
         <v>88</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="7" t="s">
         <v>59</v>
       </c>
       <c r="G31" t="s">
         <v>89</v>
       </c>
-      <c r="H31" s="4">
+      <c r="H31" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>Calvin Coolidge</v>
+      </c>
+      <c r="I31" s="4">
         <v>235000</v>
       </c>
-      <c r="I31" s="1">
-        <v>44391</v>
-      </c>
       <c r="J31" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K31" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>29</v>
       </c>
@@ -2358,23 +2512,27 @@
       <c r="E32" t="s">
         <v>90</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="7" t="s">
         <v>59</v>
       </c>
       <c r="G32" t="s">
         <v>37</v>
       </c>
-      <c r="H32" s="4">
+      <c r="H32" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>Office vacant</v>
+      </c>
+      <c r="I32" s="4">
         <v>245000</v>
       </c>
-      <c r="I32" s="1">
-        <v>44391</v>
-      </c>
       <c r="J32" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K32" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>30</v>
       </c>
@@ -2391,23 +2549,27 @@
       <c r="E33" t="s">
         <v>92</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33" s="7" t="s">
         <v>59</v>
       </c>
       <c r="G33" t="s">
         <v>93</v>
       </c>
-      <c r="H33" s="4">
+      <c r="H33" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>Charles Curtis</v>
+      </c>
+      <c r="I33" s="4">
         <v>255000</v>
       </c>
-      <c r="I33" s="1">
-        <v>44391</v>
-      </c>
       <c r="J33" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K33" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>31</v>
       </c>
@@ -2424,23 +2586,27 @@
       <c r="E34" t="s">
         <v>95</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34" s="7" t="s">
         <v>26</v>
       </c>
       <c r="G34" t="s">
         <v>96</v>
       </c>
-      <c r="H34" s="4">
+      <c r="H34" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>John Nance Garner</v>
+      </c>
+      <c r="I34" s="4">
         <v>265000</v>
       </c>
-      <c r="I34" s="1">
-        <v>44391</v>
-      </c>
       <c r="J34" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K34" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>32</v>
       </c>
@@ -2457,23 +2623,27 @@
       <c r="E35" t="s">
         <v>98</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" s="7" t="s">
         <v>26</v>
       </c>
       <c r="G35" t="s">
         <v>37</v>
       </c>
-      <c r="H35" s="4">
+      <c r="H35" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>Office vacant</v>
+      </c>
+      <c r="I35" s="4">
         <v>275000</v>
       </c>
-      <c r="I35" s="1">
-        <v>44391</v>
-      </c>
       <c r="J35" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K35" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>33</v>
       </c>
@@ -2490,23 +2660,27 @@
       <c r="E36" t="s">
         <v>100</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F36" s="7" t="s">
         <v>59</v>
       </c>
       <c r="G36" t="s">
         <v>101</v>
       </c>
-      <c r="H36" s="4">
+      <c r="H36" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>Richard Nixon</v>
+      </c>
+      <c r="I36" s="4">
         <v>285000</v>
       </c>
-      <c r="I36" s="1">
-        <v>44391</v>
-      </c>
       <c r="J36" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K36" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>34</v>
       </c>
@@ -2523,23 +2697,27 @@
       <c r="E37" t="s">
         <v>103</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F37" s="7" t="s">
         <v>26</v>
       </c>
       <c r="G37" t="s">
         <v>104</v>
       </c>
-      <c r="H37" s="4">
+      <c r="H37" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>Lyndon B. Johnson</v>
+      </c>
+      <c r="I37" s="4">
         <v>295000</v>
       </c>
-      <c r="I37" s="1">
-        <v>44391</v>
-      </c>
       <c r="J37" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K37" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>35</v>
       </c>
@@ -2556,23 +2734,27 @@
       <c r="E38" t="s">
         <v>105</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" s="7" t="s">
         <v>26</v>
       </c>
       <c r="G38" t="s">
         <v>37</v>
       </c>
-      <c r="H38" s="4">
+      <c r="H38" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>Office vacant</v>
+      </c>
+      <c r="I38" s="4">
         <v>305000</v>
       </c>
-      <c r="I38" s="1">
-        <v>44391</v>
-      </c>
       <c r="J38" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K38" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>36</v>
       </c>
@@ -2589,23 +2771,27 @@
       <c r="E39" t="s">
         <v>106</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" s="7" t="s">
         <v>59</v>
       </c>
       <c r="G39" t="s">
         <v>107</v>
       </c>
-      <c r="H39" s="4">
+      <c r="H39" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>Spiro Agnew</v>
+      </c>
+      <c r="I39" s="4">
         <v>315000</v>
       </c>
-      <c r="I39" s="1">
-        <v>44391</v>
-      </c>
       <c r="J39" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K39" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>37</v>
       </c>
@@ -2622,23 +2808,27 @@
       <c r="E40" t="s">
         <v>109</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40" s="7" t="s">
         <v>59</v>
       </c>
       <c r="G40" t="s">
         <v>37</v>
       </c>
-      <c r="H40" s="4">
+      <c r="H40" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>Office vacant</v>
+      </c>
+      <c r="I40" s="4">
         <v>325000</v>
       </c>
-      <c r="I40" s="1">
-        <v>44391</v>
-      </c>
       <c r="J40" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K40" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>38</v>
       </c>
@@ -2655,23 +2845,27 @@
       <c r="E41" t="s">
         <v>111</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" s="7" t="s">
         <v>26</v>
       </c>
       <c r="G41" t="s">
         <v>112</v>
       </c>
-      <c r="H41" s="4">
+      <c r="H41" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>Walter Mondale</v>
+      </c>
+      <c r="I41" s="4">
         <v>335000</v>
       </c>
-      <c r="I41" s="1">
-        <v>44391</v>
-      </c>
       <c r="J41" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K41" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>39</v>
       </c>
@@ -2688,23 +2882,27 @@
       <c r="E42" t="s">
         <v>114</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F42" s="7" t="s">
         <v>59</v>
       </c>
       <c r="G42" t="s">
         <v>115</v>
       </c>
-      <c r="H42" s="4">
+      <c r="H42" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>George H. W. Bush</v>
+      </c>
+      <c r="I42" s="4">
         <v>345000</v>
       </c>
-      <c r="I42" s="1">
-        <v>44391</v>
-      </c>
       <c r="J42" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K42" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>40</v>
       </c>
@@ -2721,23 +2919,27 @@
       <c r="E43" t="s">
         <v>116</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F43" s="7" t="s">
         <v>59</v>
       </c>
       <c r="G43" t="s">
         <v>117</v>
       </c>
-      <c r="H43" s="4">
+      <c r="H43" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>Dan Quayle</v>
+      </c>
+      <c r="I43" s="4">
         <v>355000</v>
       </c>
-      <c r="I43" s="1">
-        <v>44391</v>
-      </c>
       <c r="J43" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K43" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>41</v>
       </c>
@@ -2754,23 +2956,27 @@
       <c r="E44" t="s">
         <v>119</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F44" s="7" t="s">
         <v>26</v>
       </c>
       <c r="G44" t="s">
         <v>120</v>
       </c>
-      <c r="H44" s="4">
+      <c r="H44" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>Al Gore</v>
+      </c>
+      <c r="I44" s="4">
         <v>365000</v>
       </c>
-      <c r="I44" s="1">
-        <v>44391</v>
-      </c>
       <c r="J44" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K44" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>42</v>
       </c>
@@ -2787,23 +2993,27 @@
       <c r="E45" t="s">
         <v>122</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F45" s="7" t="s">
         <v>59</v>
       </c>
       <c r="G45" t="s">
         <v>123</v>
       </c>
-      <c r="H45" s="4">
+      <c r="H45" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>Dick Cheney</v>
+      </c>
+      <c r="I45" s="4">
         <v>375000</v>
       </c>
-      <c r="I45" s="1">
-        <v>44391</v>
-      </c>
       <c r="J45" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="K45" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>43</v>
       </c>
@@ -2820,23 +3030,27 @@
       <c r="E46" t="s">
         <v>125</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F46" s="7" t="s">
         <v>26</v>
       </c>
       <c r="G46" t="s">
         <v>126</v>
       </c>
-      <c r="H46" s="4">
+      <c r="H46" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>Joe Biden</v>
+      </c>
+      <c r="I46" s="4">
         <v>395000</v>
       </c>
-      <c r="I46" s="2">
-        <v>44391</v>
-      </c>
       <c r="J46" s="2">
+        <v>44391</v>
+      </c>
+      <c r="K46" s="2">
         <v>43862</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>44</v>
       </c>
@@ -2853,27 +3067,31 @@
       <c r="E47" t="s">
         <v>128</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F47" s="7" t="s">
         <v>59</v>
       </c>
       <c r="G47" t="s">
         <v>129</v>
       </c>
-      <c r="H47" s="4">
+      <c r="H47" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>Mike Pence</v>
+      </c>
+      <c r="I47" s="4">
         <v>405000</v>
       </c>
-      <c r="I47" s="2">
-        <v>44391</v>
-      </c>
       <c r="J47" s="2">
+        <v>44391</v>
+      </c>
+      <c r="K47" s="2">
         <v>43862</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H48"/>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I48"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J47" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:K47" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <dataConsolidate/>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Salary column fixed by applying Number format instead Currency format for better calculations
</commit_message>
<xml_diff>
--- a/Excel/Data Cleaning Excel Tutorial.xlsx
+++ b/Excel/Data Cleaning Excel Tutorial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milo4\Desktop\DataAnalysisLearning\Data-Analysis-Portfolio-Projects\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED3964A-8254-4DE5-9547-35A606414823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DCF11A3-265F-468B-B4EF-980D1ECE8EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -452,9 +452,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -980,13 +979,13 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1344,8 +1343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1360,19 +1359,19 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>135</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>3</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>136</v>
       </c>
       <c r="I1" s="3" t="s">
@@ -1395,24 +1394,24 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="5" t="str">
+      <c r="D2" s="4" t="str">
         <f>PROPER(C2)</f>
         <v>George Washington</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>130</v>
       </c>
       <c r="G2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="9" t="str">
+      <c r="H2" s="8" t="str">
         <f>TRIM(G2)</f>
         <v>John Adams</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="10">
         <v>5000</v>
       </c>
       <c r="J2" s="1">
@@ -1432,24 +1431,24 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="5" t="str">
+      <c r="D3" s="4" t="str">
         <f t="shared" ref="D3:D47" si="0">PROPER(C3)</f>
         <v>John Adams</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="9" t="str">
+      <c r="H3" s="8" t="str">
         <f t="shared" ref="H3:H47" si="1">TRIM(G3)</f>
         <v>Thomas Jefferson</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="10">
         <v>10000</v>
       </c>
       <c r="J3" s="1">
@@ -1469,24 +1468,24 @@
       <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="5" t="str">
+      <c r="D4" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Thomas Jefferson</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="6" t="s">
         <v>13</v>
       </c>
       <c r="G4" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="9" t="str">
+      <c r="H4" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Aaron Burr</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="10">
         <v>15000</v>
       </c>
       <c r="J4" s="1">
@@ -1506,24 +1505,24 @@
       <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="5" t="str">
+      <c r="D5" s="4" t="str">
         <f t="shared" si="0"/>
         <v>James Madison</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>13</v>
       </c>
       <c r="G5" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="9" t="str">
+      <c r="H5" s="8" t="str">
         <f t="shared" si="1"/>
         <v>George Clinton</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="10">
         <v>20000</v>
       </c>
       <c r="J5" s="1">
@@ -1543,24 +1542,24 @@
       <c r="C6" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="5" t="str">
+      <c r="D6" s="4" t="str">
         <f t="shared" si="0"/>
         <v>James Monroe</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="6" t="s">
         <v>13</v>
       </c>
       <c r="G6" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="9" t="str">
+      <c r="H6" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Daniel D. Tompkins</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="10">
         <v>25000</v>
       </c>
       <c r="J6" s="1">
@@ -1580,24 +1579,24 @@
       <c r="C7" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="5" t="str">
+      <c r="D7" s="4" t="str">
         <f t="shared" si="0"/>
         <v>John Quincy Adams</v>
       </c>
       <c r="E7" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="6" t="s">
         <v>13</v>
       </c>
       <c r="G7" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="9" t="str">
+      <c r="H7" s="8" t="str">
         <f t="shared" si="1"/>
         <v>John C. Calhoun</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="10">
         <v>30000</v>
       </c>
       <c r="J7" s="1">
@@ -1617,24 +1616,24 @@
       <c r="C8" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="5" t="str">
+      <c r="D8" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Andrew Jackson</v>
       </c>
       <c r="E8" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="6" t="s">
         <v>26</v>
       </c>
       <c r="G8" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="9" t="str">
+      <c r="H8" s="8" t="str">
         <f t="shared" si="1"/>
         <v>John C. Calhoun</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="10">
         <v>35000</v>
       </c>
       <c r="J8" s="1">
@@ -1654,24 +1653,24 @@
       <c r="C9" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="5" t="str">
+      <c r="D9" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Martin Van Buren</v>
       </c>
       <c r="E9" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="6" t="s">
         <v>26</v>
       </c>
       <c r="G9" t="s">
         <v>30</v>
       </c>
-      <c r="H9" s="9" t="str">
+      <c r="H9" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Richard Mentor Johnson</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="10">
         <v>40000</v>
       </c>
       <c r="J9" s="1">
@@ -1691,24 +1690,24 @@
       <c r="C10" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="5" t="str">
+      <c r="D10" s="4" t="str">
         <f t="shared" si="0"/>
         <v>William Henry Harrison</v>
       </c>
       <c r="E10" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="6" t="s">
         <v>33</v>
       </c>
       <c r="G10" t="s">
         <v>34</v>
       </c>
-      <c r="H10" s="9" t="str">
+      <c r="H10" s="8" t="str">
         <f t="shared" si="1"/>
         <v>John Tyler</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="10">
         <v>45000</v>
       </c>
       <c r="J10" s="1">
@@ -1728,24 +1727,24 @@
       <c r="C11" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="5" t="str">
+      <c r="D11" s="4" t="str">
         <f t="shared" si="0"/>
         <v>John Tyler</v>
       </c>
       <c r="E11" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="6" t="s">
         <v>33</v>
       </c>
       <c r="G11" t="s">
         <v>37</v>
       </c>
-      <c r="H11" s="9" t="str">
+      <c r="H11" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Office vacant</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="10">
         <v>50000</v>
       </c>
       <c r="J11" s="1">
@@ -1765,24 +1764,24 @@
       <c r="C12" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="5" t="str">
+      <c r="D12" s="4" t="str">
         <f t="shared" si="0"/>
         <v>James K. Polk</v>
       </c>
       <c r="E12" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="6" t="s">
         <v>26</v>
       </c>
       <c r="G12" t="s">
         <v>40</v>
       </c>
-      <c r="H12" s="9" t="str">
+      <c r="H12" s="8" t="str">
         <f t="shared" si="1"/>
         <v>George M. Dallas</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="10">
         <v>55000</v>
       </c>
       <c r="J12" s="1">
@@ -1802,24 +1801,24 @@
       <c r="C13" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="5" t="str">
+      <c r="D13" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Zachary Taylor</v>
       </c>
       <c r="E13" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="6" t="s">
         <v>33</v>
       </c>
       <c r="G13" t="s">
         <v>43</v>
       </c>
-      <c r="H13" s="9" t="str">
+      <c r="H13" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Millard Fillmore</v>
       </c>
-      <c r="I13" s="4">
+      <c r="I13" s="10">
         <v>60000</v>
       </c>
       <c r="J13" s="1">
@@ -1839,24 +1838,24 @@
       <c r="C14" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="5" t="str">
+      <c r="D14" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Millard Fillmore</v>
       </c>
       <c r="E14" t="s">
         <v>45</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="6" t="s">
         <v>33</v>
       </c>
       <c r="G14" t="s">
         <v>37</v>
       </c>
-      <c r="H14" s="9" t="str">
+      <c r="H14" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Office vacant</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="10">
         <v>65000</v>
       </c>
       <c r="J14" s="1">
@@ -1876,24 +1875,24 @@
       <c r="C15" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="5" t="str">
+      <c r="D15" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Franklin Pierce</v>
       </c>
       <c r="E15" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="6" t="s">
         <v>26</v>
       </c>
       <c r="G15" t="s">
         <v>48</v>
       </c>
-      <c r="H15" s="9" t="str">
+      <c r="H15" s="8" t="str">
         <f t="shared" si="1"/>
         <v>William R. King</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I15" s="10">
         <v>75000</v>
       </c>
       <c r="J15" s="1">
@@ -1913,24 +1912,24 @@
       <c r="C16" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="5" t="str">
+      <c r="D16" s="4" t="str">
         <f t="shared" si="0"/>
         <v>James Buchanan</v>
       </c>
       <c r="E16" t="s">
         <v>50</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="6" t="s">
         <v>26</v>
       </c>
       <c r="G16" t="s">
         <v>51</v>
       </c>
-      <c r="H16" s="9" t="str">
+      <c r="H16" s="8" t="str">
         <f t="shared" si="1"/>
         <v>John C. Breckinridge</v>
       </c>
-      <c r="I16" s="4">
+      <c r="I16" s="10">
         <v>85000</v>
       </c>
       <c r="J16" s="1">
@@ -1950,24 +1949,24 @@
       <c r="C17" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="5" t="str">
+      <c r="D17" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Abraham Lincoln</v>
       </c>
       <c r="E17" t="s">
         <v>53</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="6" t="s">
         <v>59</v>
       </c>
       <c r="G17" t="s">
         <v>54</v>
       </c>
-      <c r="H17" s="9" t="str">
+      <c r="H17" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Hannibal Hamlin</v>
       </c>
-      <c r="I17" s="4">
+      <c r="I17" s="10">
         <v>95000</v>
       </c>
       <c r="J17" s="1">
@@ -1987,24 +1986,24 @@
       <c r="C18" t="s">
         <v>55</v>
       </c>
-      <c r="D18" s="5" t="str">
+      <c r="D18" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Andrew Johnson</v>
       </c>
       <c r="E18" t="s">
         <v>56</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="6" t="s">
         <v>26</v>
       </c>
       <c r="G18" t="s">
         <v>37</v>
       </c>
-      <c r="H18" s="9" t="str">
+      <c r="H18" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Office vacant</v>
       </c>
-      <c r="I18" s="4">
+      <c r="I18" s="10">
         <v>105000</v>
       </c>
       <c r="J18" s="1">
@@ -2024,24 +2023,24 @@
       <c r="C19" t="s">
         <v>57</v>
       </c>
-      <c r="D19" s="5" t="str">
+      <c r="D19" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Ulysses S. Grant</v>
       </c>
       <c r="E19" t="s">
         <v>58</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="6" t="s">
         <v>59</v>
       </c>
       <c r="G19" t="s">
         <v>60</v>
       </c>
-      <c r="H19" s="9" t="str">
+      <c r="H19" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Schuyler Colfax</v>
       </c>
-      <c r="I19" s="4">
+      <c r="I19" s="10">
         <v>115000</v>
       </c>
       <c r="J19" s="1">
@@ -2061,24 +2060,24 @@
       <c r="C20" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="5" t="str">
+      <c r="D20" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Rutherford B. Hayes</v>
       </c>
       <c r="E20" t="s">
         <v>62</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="6" t="s">
         <v>59</v>
       </c>
       <c r="G20" t="s">
         <v>63</v>
       </c>
-      <c r="H20" s="9" t="str">
+      <c r="H20" s="8" t="str">
         <f t="shared" si="1"/>
         <v>William A. Wheeler</v>
       </c>
-      <c r="I20" s="4">
+      <c r="I20" s="10">
         <v>125000</v>
       </c>
       <c r="J20" s="1">
@@ -2098,24 +2097,24 @@
       <c r="C21" t="s">
         <v>64</v>
       </c>
-      <c r="D21" s="5" t="str">
+      <c r="D21" s="4" t="str">
         <f t="shared" si="0"/>
         <v>James A. Garfield</v>
       </c>
       <c r="E21" t="s">
         <v>65</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="F21" s="6" t="s">
         <v>59</v>
       </c>
       <c r="G21" t="s">
         <v>66</v>
       </c>
-      <c r="H21" s="9" t="str">
+      <c r="H21" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Chester A. Arthur</v>
       </c>
-      <c r="I21" s="4">
+      <c r="I21" s="10">
         <v>135000</v>
       </c>
       <c r="J21" s="1">
@@ -2135,24 +2134,24 @@
       <c r="C22" t="s">
         <v>66</v>
       </c>
-      <c r="D22" s="5" t="str">
+      <c r="D22" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Chester A. Arthur</v>
       </c>
       <c r="E22" t="s">
         <v>67</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="6" t="s">
         <v>59</v>
       </c>
       <c r="G22" t="s">
         <v>37</v>
       </c>
-      <c r="H22" s="9" t="str">
+      <c r="H22" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Office vacant</v>
       </c>
-      <c r="I22" s="4">
+      <c r="I22" s="10">
         <v>145000</v>
       </c>
       <c r="J22" s="1">
@@ -2172,24 +2171,24 @@
       <c r="C23" t="s">
         <v>68</v>
       </c>
-      <c r="D23" s="5" t="str">
+      <c r="D23" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Grover Cleveland</v>
       </c>
       <c r="E23" t="s">
         <v>69</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="6" t="s">
         <v>26</v>
       </c>
       <c r="G23" t="s">
         <v>70</v>
       </c>
-      <c r="H23" s="9" t="str">
+      <c r="H23" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Thomas A. Hendricks</v>
       </c>
-      <c r="I23" s="4">
+      <c r="I23" s="10">
         <v>155000</v>
       </c>
       <c r="J23" s="1">
@@ -2209,24 +2208,24 @@
       <c r="C24" t="s">
         <v>71</v>
       </c>
-      <c r="D24" s="5" t="str">
+      <c r="D24" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Benjamin Harrison</v>
       </c>
       <c r="E24" t="s">
         <v>72</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="6" t="s">
         <v>59</v>
       </c>
       <c r="G24" t="s">
         <v>73</v>
       </c>
-      <c r="H24" s="9" t="str">
+      <c r="H24" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Levi P. Morton</v>
       </c>
-      <c r="I24" s="4">
+      <c r="I24" s="10">
         <v>165000</v>
       </c>
       <c r="J24" s="1">
@@ -2246,24 +2245,24 @@
       <c r="C25" t="s">
         <v>68</v>
       </c>
-      <c r="D25" s="5" t="str">
+      <c r="D25" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Grover Cleveland</v>
       </c>
       <c r="E25" t="s">
         <v>74</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F25" s="6" t="s">
         <v>26</v>
       </c>
       <c r="G25" t="s">
         <v>75</v>
       </c>
-      <c r="H25" s="9" t="str">
+      <c r="H25" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Adlai Stevenson</v>
       </c>
-      <c r="I25" s="4">
+      <c r="I25" s="10">
         <v>175000</v>
       </c>
       <c r="J25" s="1">
@@ -2283,24 +2282,24 @@
       <c r="C26" t="s">
         <v>76</v>
       </c>
-      <c r="D26" s="5" t="str">
+      <c r="D26" s="4" t="str">
         <f t="shared" si="0"/>
         <v>William Mckinley</v>
       </c>
       <c r="E26" t="s">
         <v>77</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="F26" s="6" t="s">
         <v>59</v>
       </c>
       <c r="G26" t="s">
         <v>78</v>
       </c>
-      <c r="H26" s="9" t="str">
+      <c r="H26" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Garret Hobart</v>
       </c>
-      <c r="I26" s="4">
+      <c r="I26" s="10">
         <v>185000</v>
       </c>
       <c r="J26" s="1">
@@ -2320,24 +2319,24 @@
       <c r="C27" t="s">
         <v>79</v>
       </c>
-      <c r="D27" s="5" t="str">
+      <c r="D27" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Theodore Roosevelt</v>
       </c>
       <c r="E27" t="s">
         <v>80</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="F27" s="6" t="s">
         <v>59</v>
       </c>
       <c r="G27" t="s">
         <v>37</v>
       </c>
-      <c r="H27" s="9" t="str">
+      <c r="H27" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Office vacant</v>
       </c>
-      <c r="I27" s="4">
+      <c r="I27" s="10">
         <v>195000</v>
       </c>
       <c r="J27" s="1">
@@ -2357,24 +2356,24 @@
       <c r="C28" t="s">
         <v>81</v>
       </c>
-      <c r="D28" s="5" t="str">
+      <c r="D28" s="4" t="str">
         <f t="shared" si="0"/>
         <v>William Howard Taft</v>
       </c>
       <c r="E28" t="s">
         <v>82</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F28" s="6" t="s">
         <v>59</v>
       </c>
       <c r="G28" t="s">
         <v>83</v>
       </c>
-      <c r="H28" s="9" t="str">
+      <c r="H28" s="8" t="str">
         <f t="shared" si="1"/>
         <v>James S. Sherman</v>
       </c>
-      <c r="I28" s="4">
+      <c r="I28" s="10">
         <v>205000</v>
       </c>
       <c r="J28" s="1">
@@ -2394,24 +2393,24 @@
       <c r="C29" t="s">
         <v>84</v>
       </c>
-      <c r="D29" s="5" t="str">
+      <c r="D29" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Woodrow Wilson</v>
       </c>
       <c r="E29" t="s">
         <v>85</v>
       </c>
-      <c r="F29" s="7" t="s">
+      <c r="F29" s="6" t="s">
         <v>26</v>
       </c>
       <c r="G29" t="s">
         <v>86</v>
       </c>
-      <c r="H29" s="9" t="str">
+      <c r="H29" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Thomas R. Marshall</v>
       </c>
-      <c r="I29" s="4">
+      <c r="I29" s="10">
         <v>225000</v>
       </c>
       <c r="J29" s="1">
@@ -2431,24 +2430,24 @@
       <c r="C30" t="s">
         <v>84</v>
       </c>
-      <c r="D30" s="5" t="str">
+      <c r="D30" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Woodrow Wilson</v>
       </c>
       <c r="E30" t="s">
         <v>85</v>
       </c>
-      <c r="F30" s="7" t="s">
+      <c r="F30" s="6" t="s">
         <v>131</v>
       </c>
       <c r="G30" t="s">
         <v>86</v>
       </c>
-      <c r="H30" s="9" t="str">
+      <c r="H30" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Thomas R. Marshall</v>
       </c>
-      <c r="I30" s="4">
+      <c r="I30" s="10">
         <v>225000</v>
       </c>
       <c r="J30" s="1">
@@ -2468,24 +2467,24 @@
       <c r="C31" t="s">
         <v>87</v>
       </c>
-      <c r="D31" s="5" t="str">
+      <c r="D31" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Warren G. Harding</v>
       </c>
       <c r="E31" t="s">
         <v>88</v>
       </c>
-      <c r="F31" s="7" t="s">
+      <c r="F31" s="6" t="s">
         <v>59</v>
       </c>
       <c r="G31" t="s">
         <v>89</v>
       </c>
-      <c r="H31" s="9" t="str">
+      <c r="H31" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Calvin Coolidge</v>
       </c>
-      <c r="I31" s="4">
+      <c r="I31" s="10">
         <v>235000</v>
       </c>
       <c r="J31" s="1">
@@ -2505,24 +2504,24 @@
       <c r="C32" t="s">
         <v>89</v>
       </c>
-      <c r="D32" s="5" t="str">
+      <c r="D32" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Calvin Coolidge</v>
       </c>
       <c r="E32" t="s">
         <v>90</v>
       </c>
-      <c r="F32" s="7" t="s">
+      <c r="F32" s="6" t="s">
         <v>59</v>
       </c>
       <c r="G32" t="s">
         <v>37</v>
       </c>
-      <c r="H32" s="9" t="str">
+      <c r="H32" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Office vacant</v>
       </c>
-      <c r="I32" s="4">
+      <c r="I32" s="10">
         <v>245000</v>
       </c>
       <c r="J32" s="1">
@@ -2542,24 +2541,24 @@
       <c r="C33" t="s">
         <v>91</v>
       </c>
-      <c r="D33" s="5" t="str">
+      <c r="D33" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Herbert Hoover</v>
       </c>
       <c r="E33" t="s">
         <v>92</v>
       </c>
-      <c r="F33" s="7" t="s">
+      <c r="F33" s="6" t="s">
         <v>59</v>
       </c>
       <c r="G33" t="s">
         <v>93</v>
       </c>
-      <c r="H33" s="9" t="str">
+      <c r="H33" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Charles Curtis</v>
       </c>
-      <c r="I33" s="4">
+      <c r="I33" s="10">
         <v>255000</v>
       </c>
       <c r="J33" s="1">
@@ -2579,24 +2578,24 @@
       <c r="C34" t="s">
         <v>94</v>
       </c>
-      <c r="D34" s="5" t="str">
+      <c r="D34" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Franklin D. Roosevelt</v>
       </c>
       <c r="E34" t="s">
         <v>95</v>
       </c>
-      <c r="F34" s="7" t="s">
+      <c r="F34" s="6" t="s">
         <v>26</v>
       </c>
       <c r="G34" t="s">
         <v>96</v>
       </c>
-      <c r="H34" s="9" t="str">
+      <c r="H34" s="8" t="str">
         <f t="shared" si="1"/>
         <v>John Nance Garner</v>
       </c>
-      <c r="I34" s="4">
+      <c r="I34" s="10">
         <v>265000</v>
       </c>
       <c r="J34" s="1">
@@ -2616,24 +2615,24 @@
       <c r="C35" t="s">
         <v>97</v>
       </c>
-      <c r="D35" s="5" t="str">
+      <c r="D35" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Harry S. Truman</v>
       </c>
       <c r="E35" t="s">
         <v>98</v>
       </c>
-      <c r="F35" s="7" t="s">
+      <c r="F35" s="6" t="s">
         <v>26</v>
       </c>
       <c r="G35" t="s">
         <v>37</v>
       </c>
-      <c r="H35" s="9" t="str">
+      <c r="H35" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Office vacant</v>
       </c>
-      <c r="I35" s="4">
+      <c r="I35" s="10">
         <v>275000</v>
       </c>
       <c r="J35" s="1">
@@ -2653,24 +2652,24 @@
       <c r="C36" t="s">
         <v>99</v>
       </c>
-      <c r="D36" s="5" t="str">
+      <c r="D36" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Dwight D. Eisenhower</v>
       </c>
       <c r="E36" t="s">
         <v>100</v>
       </c>
-      <c r="F36" s="7" t="s">
+      <c r="F36" s="6" t="s">
         <v>59</v>
       </c>
       <c r="G36" t="s">
         <v>101</v>
       </c>
-      <c r="H36" s="9" t="str">
+      <c r="H36" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Richard Nixon</v>
       </c>
-      <c r="I36" s="4">
+      <c r="I36" s="10">
         <v>285000</v>
       </c>
       <c r="J36" s="1">
@@ -2690,24 +2689,24 @@
       <c r="C37" t="s">
         <v>102</v>
       </c>
-      <c r="D37" s="5" t="str">
+      <c r="D37" s="4" t="str">
         <f t="shared" si="0"/>
         <v>John F. Kennedy</v>
       </c>
       <c r="E37" t="s">
         <v>103</v>
       </c>
-      <c r="F37" s="7" t="s">
+      <c r="F37" s="6" t="s">
         <v>26</v>
       </c>
       <c r="G37" t="s">
         <v>104</v>
       </c>
-      <c r="H37" s="9" t="str">
+      <c r="H37" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Lyndon B. Johnson</v>
       </c>
-      <c r="I37" s="4">
+      <c r="I37" s="10">
         <v>295000</v>
       </c>
       <c r="J37" s="1">
@@ -2727,24 +2726,24 @@
       <c r="C38" t="s">
         <v>104</v>
       </c>
-      <c r="D38" s="5" t="str">
+      <c r="D38" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Lyndon B. Johnson</v>
       </c>
       <c r="E38" t="s">
         <v>105</v>
       </c>
-      <c r="F38" s="7" t="s">
+      <c r="F38" s="6" t="s">
         <v>26</v>
       </c>
       <c r="G38" t="s">
         <v>37</v>
       </c>
-      <c r="H38" s="9" t="str">
+      <c r="H38" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Office vacant</v>
       </c>
-      <c r="I38" s="4">
+      <c r="I38" s="10">
         <v>305000</v>
       </c>
       <c r="J38" s="1">
@@ -2764,24 +2763,24 @@
       <c r="C39" t="s">
         <v>101</v>
       </c>
-      <c r="D39" s="5" t="str">
+      <c r="D39" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Richard Nixon</v>
       </c>
       <c r="E39" t="s">
         <v>106</v>
       </c>
-      <c r="F39" s="7" t="s">
+      <c r="F39" s="6" t="s">
         <v>59</v>
       </c>
       <c r="G39" t="s">
         <v>107</v>
       </c>
-      <c r="H39" s="9" t="str">
+      <c r="H39" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Spiro Agnew</v>
       </c>
-      <c r="I39" s="4">
+      <c r="I39" s="10">
         <v>315000</v>
       </c>
       <c r="J39" s="1">
@@ -2801,24 +2800,24 @@
       <c r="C40" t="s">
         <v>108</v>
       </c>
-      <c r="D40" s="5" t="str">
+      <c r="D40" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Gerald Ford</v>
       </c>
       <c r="E40" t="s">
         <v>109</v>
       </c>
-      <c r="F40" s="7" t="s">
+      <c r="F40" s="6" t="s">
         <v>59</v>
       </c>
       <c r="G40" t="s">
         <v>37</v>
       </c>
-      <c r="H40" s="9" t="str">
+      <c r="H40" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Office vacant</v>
       </c>
-      <c r="I40" s="4">
+      <c r="I40" s="10">
         <v>325000</v>
       </c>
       <c r="J40" s="1">
@@ -2838,24 +2837,24 @@
       <c r="C41" t="s">
         <v>110</v>
       </c>
-      <c r="D41" s="5" t="str">
+      <c r="D41" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Jimmy Carter</v>
       </c>
       <c r="E41" t="s">
         <v>111</v>
       </c>
-      <c r="F41" s="7" t="s">
+      <c r="F41" s="6" t="s">
         <v>26</v>
       </c>
       <c r="G41" t="s">
         <v>112</v>
       </c>
-      <c r="H41" s="9" t="str">
+      <c r="H41" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Walter Mondale</v>
       </c>
-      <c r="I41" s="4">
+      <c r="I41" s="10">
         <v>335000</v>
       </c>
       <c r="J41" s="1">
@@ -2875,24 +2874,24 @@
       <c r="C42" t="s">
         <v>113</v>
       </c>
-      <c r="D42" s="5" t="str">
+      <c r="D42" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Ronald Reagan</v>
       </c>
       <c r="E42" t="s">
         <v>114</v>
       </c>
-      <c r="F42" s="7" t="s">
+      <c r="F42" s="6" t="s">
         <v>59</v>
       </c>
       <c r="G42" t="s">
         <v>115</v>
       </c>
-      <c r="H42" s="9" t="str">
+      <c r="H42" s="8" t="str">
         <f t="shared" si="1"/>
         <v>George H. W. Bush</v>
       </c>
-      <c r="I42" s="4">
+      <c r="I42" s="10">
         <v>345000</v>
       </c>
       <c r="J42" s="1">
@@ -2912,24 +2911,24 @@
       <c r="C43" t="s">
         <v>115</v>
       </c>
-      <c r="D43" s="5" t="str">
+      <c r="D43" s="4" t="str">
         <f t="shared" si="0"/>
         <v>George H. W. Bush</v>
       </c>
       <c r="E43" t="s">
         <v>116</v>
       </c>
-      <c r="F43" s="7" t="s">
+      <c r="F43" s="6" t="s">
         <v>59</v>
       </c>
       <c r="G43" t="s">
         <v>117</v>
       </c>
-      <c r="H43" s="9" t="str">
+      <c r="H43" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Dan Quayle</v>
       </c>
-      <c r="I43" s="4">
+      <c r="I43" s="10">
         <v>355000</v>
       </c>
       <c r="J43" s="1">
@@ -2949,24 +2948,24 @@
       <c r="C44" t="s">
         <v>118</v>
       </c>
-      <c r="D44" s="5" t="str">
+      <c r="D44" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Bill Clinton</v>
       </c>
       <c r="E44" t="s">
         <v>119</v>
       </c>
-      <c r="F44" s="7" t="s">
+      <c r="F44" s="6" t="s">
         <v>26</v>
       </c>
       <c r="G44" t="s">
         <v>120</v>
       </c>
-      <c r="H44" s="9" t="str">
+      <c r="H44" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Al Gore</v>
       </c>
-      <c r="I44" s="4">
+      <c r="I44" s="10">
         <v>365000</v>
       </c>
       <c r="J44" s="1">
@@ -2986,24 +2985,24 @@
       <c r="C45" t="s">
         <v>121</v>
       </c>
-      <c r="D45" s="5" t="str">
+      <c r="D45" s="4" t="str">
         <f t="shared" si="0"/>
         <v>George W. Bush</v>
       </c>
       <c r="E45" t="s">
         <v>122</v>
       </c>
-      <c r="F45" s="7" t="s">
+      <c r="F45" s="6" t="s">
         <v>59</v>
       </c>
       <c r="G45" t="s">
         <v>123</v>
       </c>
-      <c r="H45" s="9" t="str">
+      <c r="H45" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Dick Cheney</v>
       </c>
-      <c r="I45" s="4">
+      <c r="I45" s="10">
         <v>375000</v>
       </c>
       <c r="J45" s="1">
@@ -3023,24 +3022,24 @@
       <c r="C46" t="s">
         <v>124</v>
       </c>
-      <c r="D46" s="5" t="str">
+      <c r="D46" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Barack Obama</v>
       </c>
       <c r="E46" t="s">
         <v>125</v>
       </c>
-      <c r="F46" s="7" t="s">
+      <c r="F46" s="6" t="s">
         <v>26</v>
       </c>
       <c r="G46" t="s">
         <v>126</v>
       </c>
-      <c r="H46" s="9" t="str">
+      <c r="H46" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Joe Biden</v>
       </c>
-      <c r="I46" s="4">
+      <c r="I46" s="10">
         <v>395000</v>
       </c>
       <c r="J46" s="2">
@@ -3060,24 +3059,24 @@
       <c r="C47" t="s">
         <v>127</v>
       </c>
-      <c r="D47" s="5" t="str">
+      <c r="D47" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Donald Trump</v>
       </c>
       <c r="E47" t="s">
         <v>128</v>
       </c>
-      <c r="F47" s="7" t="s">
+      <c r="F47" s="6" t="s">
         <v>59</v>
       </c>
       <c r="G47" t="s">
         <v>129</v>
       </c>
-      <c r="H47" s="9" t="str">
+      <c r="H47" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Mike Pence</v>
       </c>
-      <c r="I47" s="4">
+      <c r="I47" s="10">
         <v>405000</v>
       </c>
       <c r="J47" s="2">

</xml_diff>